<commit_message>
more changes to acronyms file
</commit_message>
<xml_diff>
--- a/src/main/resources/dictionaries/Acronyms.xlsx
+++ b/src/main/resources/dictionaries/Acronyms.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="460">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="470">
   <si>
     <t>#</t>
   </si>
@@ -290,6 +290,9 @@
     <t>#Satellites / Satellite Instruments - This is from GAW needs more work.</t>
   </si>
   <si>
+    <t>NNP-SATELLITE</t>
+  </si>
+  <si>
     <t>CLAES</t>
   </si>
   <si>
@@ -350,6 +353,9 @@
     <t>Global Atmospheric Watch</t>
   </si>
   <si>
+    <t>NNP-NETWORK</t>
+  </si>
+  <si>
     <t>EMEP </t>
   </si>
   <si>
@@ -518,7 +524,7 @@
     <t>#International programmes or conventions</t>
   </si>
   <si>
-    <t>NNP-Program</t>
+    <t>NNP-PROGRAMME</t>
   </si>
   <si>
     <t>CACGP</t>
@@ -749,6 +755,9 @@
     <t># Field Campaigns - from GAW acronymns</t>
   </si>
   <si>
+    <t>NNP-CAMPAIGN</t>
+  </si>
+  <si>
     <t>ACE </t>
   </si>
   <si>
@@ -872,6 +881,9 @@
     <t>#Other Institutes / committees</t>
   </si>
   <si>
+    <t>NNP-INSTITUTE</t>
+  </si>
+  <si>
     <t>ASRC-SUNY </t>
   </si>
   <si>
@@ -1202,34 +1214,52 @@
     <t>#units:</t>
   </si>
   <si>
+    <t>NN-PPM</t>
+  </si>
+  <si>
     <t>ppm</t>
   </si>
   <si>
     <t>units: parts per million</t>
   </si>
   <si>
+    <t>NN-PPB</t>
+  </si>
+  <si>
     <t>ppb</t>
   </si>
   <si>
     <t>units: parts per billion</t>
   </si>
   <si>
+    <t>NN-PPT</t>
+  </si>
+  <si>
     <t>ppt</t>
   </si>
   <si>
     <t>units: parts per trillion</t>
   </si>
   <si>
+    <t>NN-PPMV</t>
+  </si>
+  <si>
     <t>ppmv</t>
   </si>
   <si>
     <t>units: parts per million by volume</t>
   </si>
   <si>
+    <t>NN-PPBV</t>
+  </si>
+  <si>
     <t>ppbv</t>
   </si>
   <si>
     <t>units: parts per billion by volume</t>
+  </si>
+  <si>
+    <t>NN-PPTV</t>
   </si>
   <si>
     <t>pptv</t>
@@ -2074,82 +2104,109 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="51">
+      <c r="A51" s="0" t="s">
+        <v>91</v>
+      </c>
       <c r="B51" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="52">
+      <c r="A52" s="0" t="str">
+        <f aca="false">A51</f>
+        <v>NNP-SATELLITE</v>
+      </c>
       <c r="B52" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="53">
+      <c r="A53" s="0" t="str">
+        <f aca="false">A52</f>
+        <v>NNP-SATELLITE</v>
+      </c>
       <c r="B53" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="54">
+      <c r="A54" s="0" t="str">
+        <f aca="false">A53</f>
+        <v>NNP-SATELLITE</v>
+      </c>
       <c r="B54" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D54" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="55">
+      <c r="A55" s="0" t="str">
+        <f aca="false">A54</f>
+        <v>NNP-SATELLITE</v>
+      </c>
       <c r="B55" s="0" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
       <c r="F55" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="56">
+      <c r="A56" s="0" t="str">
+        <f aca="false">A55</f>
+        <v>NNP-SATELLITE</v>
+      </c>
       <c r="B56" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="57">
+      <c r="A57" s="0" t="str">
+        <f aca="false">A56</f>
+        <v>NNP-SATELLITE</v>
+      </c>
       <c r="B57" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
@@ -2158,227 +2215,306 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="60">
       <c r="B60" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="61">
       <c r="B61" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="62">
+      <c r="A62" s="0" t="s">
+        <v>112</v>
+      </c>
       <c r="B62" s="0" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="63">
+      <c r="A63" s="0" t="str">
+        <f aca="false">A62</f>
+        <v>NNP-NETWORK</v>
+      </c>
       <c r="B63" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="64">
+      <c r="A64" s="0" t="str">
+        <f aca="false">A63</f>
+        <v>NNP-NETWORK</v>
+      </c>
       <c r="B64" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C64" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="D64" s="0" t="s">
         <v>117</v>
       </c>
-      <c r="D64" s="0" t="s">
-        <v>115</v>
-      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="65">
+      <c r="A65" s="0" t="str">
+        <f aca="false">A64</f>
+        <v>NNP-NETWORK</v>
+      </c>
       <c r="B65" s="0" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="66">
+      <c r="A66" s="0" t="str">
+        <f aca="false">A65</f>
+        <v>NNP-NETWORK</v>
+      </c>
       <c r="B66" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="67">
+      <c r="A67" s="0" t="str">
+        <f aca="false">A66</f>
+        <v>NNP-NETWORK</v>
+      </c>
       <c r="B67" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="E67" s="0" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="F67" s="0" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="68">
+      <c r="A68" s="0" t="str">
+        <f aca="false">A67</f>
+        <v>NNP-NETWORK</v>
+      </c>
       <c r="B68" s="0" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="69">
+      <c r="A69" s="0" t="str">
+        <f aca="false">A68</f>
+        <v>NNP-NETWORK</v>
+      </c>
       <c r="B69" s="0" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="70">
+      <c r="A70" s="0" t="str">
+        <f aca="false">A69</f>
+        <v>NNP-NETWORK</v>
+      </c>
       <c r="B70" s="0" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="71">
+      <c r="A71" s="0" t="str">
+        <f aca="false">A70</f>
+        <v>NNP-NETWORK</v>
+      </c>
       <c r="B71" s="0" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D71" s="0" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="E71" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="72">
+      <c r="A72" s="0" t="str">
+        <f aca="false">A71</f>
+        <v>NNP-NETWORK</v>
+      </c>
       <c r="B72" s="0" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D72" s="0" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="H72" s="2"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="73">
+      <c r="A73" s="0" t="str">
+        <f aca="false">A72</f>
+        <v>NNP-NETWORK</v>
+      </c>
       <c r="B73" s="0" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D73" s="0" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="74">
+      <c r="A74" s="0" t="str">
+        <f aca="false">A73</f>
+        <v>NNP-NETWORK</v>
+      </c>
       <c r="B74" s="0" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="75">
+      <c r="A75" s="0" t="str">
+        <f aca="false">A74</f>
+        <v>NNP-NETWORK</v>
+      </c>
       <c r="B75" s="0" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D75" s="0" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="76">
+      <c r="A76" s="0" t="str">
+        <f aca="false">A75</f>
+        <v>NNP-NETWORK</v>
+      </c>
       <c r="B76" s="0" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="D76" s="0" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="77">
+      <c r="A77" s="0" t="str">
+        <f aca="false">A76</f>
+        <v>NNP-NETWORK</v>
+      </c>
       <c r="B77" s="0" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="D77" s="0" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="78">
+      <c r="A78" s="0" t="str">
+        <f aca="false">A77</f>
+        <v>NNP-NETWORK</v>
+      </c>
       <c r="B78" s="0" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D78" s="0" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="79">
+      <c r="A79" s="0" t="str">
+        <f aca="false">A78</f>
+        <v>NNP-NETWORK</v>
+      </c>
       <c r="B79" s="0" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D79" s="0" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="80">
+      <c r="A80" s="0" t="str">
+        <f aca="false">A79</f>
+        <v>NNP-NETWORK</v>
+      </c>
       <c r="B80" s="0" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="D80" s="0" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="81">
+      <c r="A81" s="0" t="str">
+        <f aca="false">A80</f>
+        <v>NNP-NETWORK</v>
+      </c>
       <c r="B81" s="0" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="D81" s="0" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="82">
@@ -2389,839 +2525,1216 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="85">
       <c r="B85" s="0" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="86">
       <c r="A86" s="0" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="D86" s="1"/>
       <c r="E86" s="1"/>
       <c r="F86" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="87">
+      <c r="A87" s="0" t="str">
+        <f aca="false">A86</f>
+        <v>NNP-PROGRAMME</v>
+      </c>
       <c r="B87" s="0" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="D87" s="1"/>
       <c r="E87" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="88">
+      <c r="A88" s="0" t="str">
+        <f aca="false">A87</f>
+        <v>NNP-PROGRAMME</v>
+      </c>
       <c r="B88" s="0" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="D88" s="1"/>
       <c r="E88" s="1"/>
       <c r="F88" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="89">
+      <c r="A89" s="0" t="str">
+        <f aca="false">A88</f>
+        <v>NNP-PROGRAMME</v>
+      </c>
       <c r="B89" s="0" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C89" s="0" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="90">
+      <c r="A90" s="0" t="str">
+        <f aca="false">A89</f>
+        <v>NNP-PROGRAMME</v>
+      </c>
       <c r="B90" s="0" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="91">
+      <c r="A91" s="0" t="str">
+        <f aca="false">A90</f>
+        <v>NNP-PROGRAMME</v>
+      </c>
       <c r="B91" s="0" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C91" s="0" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="92">
+      <c r="A92" s="0" t="str">
+        <f aca="false">A91</f>
+        <v>NNP-PROGRAMME</v>
+      </c>
       <c r="B92" s="0" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C92" s="0" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="93">
+      <c r="A93" s="0" t="str">
+        <f aca="false">A92</f>
+        <v>NNP-PROGRAMME</v>
+      </c>
       <c r="B93" s="0" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C93" s="0" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="94">
+      <c r="A94" s="0" t="str">
+        <f aca="false">A93</f>
+        <v>NNP-PROGRAMME</v>
+      </c>
       <c r="B94" s="0" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C94" s="0" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="95">
+      <c r="A95" s="0" t="str">
+        <f aca="false">A94</f>
+        <v>NNP-PROGRAMME</v>
+      </c>
       <c r="B95" s="0" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="C95" s="0" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="96">
+      <c r="A96" s="0" t="str">
+        <f aca="false">A95</f>
+        <v>NNP-PROGRAMME</v>
+      </c>
       <c r="B96" s="0" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="C96" s="0" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="97">
+      <c r="A97" s="0" t="str">
+        <f aca="false">A96</f>
+        <v>NNP-PROGRAMME</v>
+      </c>
       <c r="B97" s="0" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C97" s="0" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="98">
+      <c r="A98" s="0" t="str">
+        <f aca="false">A97</f>
+        <v>NNP-PROGRAMME</v>
+      </c>
       <c r="B98" s="0" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C98" s="0" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="99">
+      <c r="A99" s="0" t="str">
+        <f aca="false">A98</f>
+        <v>NNP-PROGRAMME</v>
+      </c>
       <c r="B99" s="0" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="D99" s="1"/>
       <c r="E99" s="1"/>
       <c r="F99" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="100">
+      <c r="A100" s="0" t="str">
+        <f aca="false">A99</f>
+        <v>NNP-PROGRAMME</v>
+      </c>
       <c r="B100" s="0" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="D100" s="1"/>
       <c r="E100" s="1"/>
       <c r="F100" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="101">
+      <c r="A101" s="0" t="str">
+        <f aca="false">A100</f>
+        <v>NNP-PROGRAMME</v>
+      </c>
       <c r="B101" s="0" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D101" s="1"/>
       <c r="E101" s="1"/>
       <c r="F101" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="102">
+      <c r="A102" s="0" t="str">
+        <f aca="false">A101</f>
+        <v>NNP-PROGRAMME</v>
+      </c>
       <c r="B102" s="0" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="D102" s="1"/>
       <c r="E102" s="1"/>
       <c r="F102" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="103">
+      <c r="A103" s="0" t="str">
+        <f aca="false">A102</f>
+        <v>NNP-PROGRAMME</v>
+      </c>
       <c r="B103" s="0" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="D103" s="1"/>
       <c r="E103" s="1"/>
       <c r="F103" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="104">
+      <c r="A104" s="0" t="str">
+        <f aca="false">A103</f>
+        <v>NNP-PROGRAMME</v>
+      </c>
       <c r="B104" s="0" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C104" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="105">
+      <c r="A105" s="0" t="str">
+        <f aca="false">A104</f>
+        <v>NNP-PROGRAMME</v>
+      </c>
       <c r="B105" s="0" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C105" s="0" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="106">
+      <c r="A106" s="0" t="str">
+        <f aca="false">A105</f>
+        <v>NNP-PROGRAMME</v>
+      </c>
       <c r="B106" s="0" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="C106" s="0" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="107">
+      <c r="A107" s="0" t="str">
+        <f aca="false">A106</f>
+        <v>NNP-PROGRAMME</v>
+      </c>
       <c r="B107" s="0" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="C107" s="0" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="108">
+      <c r="A108" s="0" t="str">
+        <f aca="false">A107</f>
+        <v>NNP-PROGRAMME</v>
+      </c>
       <c r="B108" s="0" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="C108" s="0" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="109">
+      <c r="A109" s="0" t="str">
+        <f aca="false">A108</f>
+        <v>NNP-PROGRAMME</v>
+      </c>
       <c r="B109" s="0" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="C109" s="0" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="110">
+      <c r="A110" s="0" t="str">
+        <f aca="false">A109</f>
+        <v>NNP-PROGRAMME</v>
+      </c>
       <c r="B110" s="0" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="C110" s="0" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="111">
+      <c r="A111" s="0" t="str">
+        <f aca="false">A110</f>
+        <v>NNP-PROGRAMME</v>
+      </c>
       <c r="B111" s="0" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="C111" s="0" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="112">
+      <c r="A112" s="0" t="str">
+        <f aca="false">A111</f>
+        <v>NNP-PROGRAMME</v>
+      </c>
       <c r="B112" s="0" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="C112" s="0" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="113">
+      <c r="A113" s="0" t="str">
+        <f aca="false">A112</f>
+        <v>NNP-PROGRAMME</v>
+      </c>
       <c r="B113" s="0" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="C113" s="0" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="114">
+      <c r="A114" s="0" t="str">
+        <f aca="false">A113</f>
+        <v>NNP-PROGRAMME</v>
+      </c>
       <c r="B114" s="0" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="C114" s="0" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="115">
+      <c r="A115" s="0" t="str">
+        <f aca="false">A114</f>
+        <v>NNP-PROGRAMME</v>
+      </c>
       <c r="B115" s="0" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="C115" s="0" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="116">
+      <c r="A116" s="0" t="str">
+        <f aca="false">A115</f>
+        <v>NNP-PROGRAMME</v>
+      </c>
       <c r="B116" s="0" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C116" s="0" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="117">
+      <c r="A117" s="0" t="str">
+        <f aca="false">A116</f>
+        <v>NNP-PROGRAMME</v>
+      </c>
       <c r="B117" s="0" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C117" s="0" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="118">
+      <c r="A118" s="0" t="str">
+        <f aca="false">A117</f>
+        <v>NNP-PROGRAMME</v>
+      </c>
       <c r="B118" s="0" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="C118" s="0" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="119">
+      <c r="A119" s="0" t="str">
+        <f aca="false">A118</f>
+        <v>NNP-PROGRAMME</v>
+      </c>
       <c r="B119" s="0" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="C119" s="0" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="120">
+      <c r="A120" s="0" t="str">
+        <f aca="false">A119</f>
+        <v>NNP-PROGRAMME</v>
+      </c>
       <c r="B120" s="0" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="C120" s="0" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="121">
+      <c r="A121" s="0" t="str">
+        <f aca="false">A120</f>
+        <v>NNP-PROGRAMME</v>
+      </c>
       <c r="B121" s="0" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="C121" s="0" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="122">
+      <c r="A122" s="0" t="str">
+        <f aca="false">A121</f>
+        <v>NNP-PROGRAMME</v>
+      </c>
       <c r="B122" s="0" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="C122" s="0" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="126">
       <c r="B126" s="0" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="128">
       <c r="B128" s="0" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="129">
+      <c r="A129" s="0" t="s">
+        <v>246</v>
+      </c>
       <c r="B129" s="0" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="C129" s="0" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="130">
+      <c r="A130" s="0" t="str">
+        <f aca="false">A129</f>
+        <v>NNP-CAMPAIGN</v>
+      </c>
       <c r="B130" s="0" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="C130" s="0" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="131">
+      <c r="A131" s="0" t="str">
+        <f aca="false">A130</f>
+        <v>NNP-CAMPAIGN</v>
+      </c>
       <c r="B131" s="0" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="C131" s="0" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="132">
+      <c r="A132" s="0" t="str">
+        <f aca="false">A131</f>
+        <v>NNP-CAMPAIGN</v>
+      </c>
       <c r="B132" s="0" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="C132" s="0" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="133">
+      <c r="A133" s="0" t="str">
+        <f aca="false">A132</f>
+        <v>NNP-CAMPAIGN</v>
+      </c>
       <c r="B133" s="0" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="C133" s="0" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="134">
+      <c r="A134" s="0" t="str">
+        <f aca="false">A133</f>
+        <v>NNP-CAMPAIGN</v>
+      </c>
       <c r="B134" s="0" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C134" s="0" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="135">
+      <c r="A135" s="0" t="str">
+        <f aca="false">A134</f>
+        <v>NNP-CAMPAIGN</v>
+      </c>
       <c r="B135" s="0" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="C135" s="0" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="136">
+      <c r="A136" s="0" t="str">
+        <f aca="false">A135</f>
+        <v>NNP-CAMPAIGN</v>
+      </c>
       <c r="B136" s="0" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="C136" s="0" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="137">
+      <c r="A137" s="0" t="str">
+        <f aca="false">A136</f>
+        <v>NNP-CAMPAIGN</v>
+      </c>
       <c r="B137" s="0" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="C137" s="0" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="138">
+      <c r="A138" s="0" t="str">
+        <f aca="false">A137</f>
+        <v>NNP-CAMPAIGN</v>
+      </c>
       <c r="B138" s="0" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="C138" s="0" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="139">
+      <c r="A139" s="0" t="str">
+        <f aca="false">A138</f>
+        <v>NNP-CAMPAIGN</v>
+      </c>
       <c r="B139" s="0" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C139" s="0" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="140">
+      <c r="A140" s="0" t="str">
+        <f aca="false">A139</f>
+        <v>NNP-CAMPAIGN</v>
+      </c>
       <c r="B140" s="0" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="C140" s="0" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="141">
+      <c r="A141" s="0" t="str">
+        <f aca="false">A140</f>
+        <v>NNP-CAMPAIGN</v>
+      </c>
       <c r="B141" s="0" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="C141" s="0" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="142">
+      <c r="A142" s="0" t="str">
+        <f aca="false">A141</f>
+        <v>NNP-CAMPAIGN</v>
+      </c>
       <c r="B142" s="0" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="C142" s="0" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="143">
+      <c r="A143" s="0" t="str">
+        <f aca="false">A142</f>
+        <v>NNP-CAMPAIGN</v>
+      </c>
       <c r="B143" s="0" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="C143" s="0" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="144">
+      <c r="A144" s="0" t="str">
+        <f aca="false">A143</f>
+        <v>NNP-CAMPAIGN</v>
+      </c>
       <c r="B144" s="0" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="C144" s="0" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="145">
+      <c r="A145" s="0" t="str">
+        <f aca="false">A144</f>
+        <v>NNP-CAMPAIGN</v>
+      </c>
       <c r="B145" s="0" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="C145" s="0" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="146">
+      <c r="A146" s="0" t="str">
+        <f aca="false">A145</f>
+        <v>NNP-CAMPAIGN</v>
+      </c>
       <c r="B146" s="0" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="C146" s="0" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="147">
+      <c r="A147" s="0" t="str">
+        <f aca="false">A146</f>
+        <v>NNP-CAMPAIGN</v>
+      </c>
       <c r="B147" s="0" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="C147" s="0" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="148">
+      <c r="A148" s="0" t="str">
+        <f aca="false">A147</f>
+        <v>NNP-CAMPAIGN</v>
+      </c>
       <c r="B148" s="0" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="C148" s="0" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="150">
       <c r="B150" s="0" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="152">
+      <c r="A152" s="0" t="s">
+        <v>288</v>
+      </c>
       <c r="B152" s="0" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="C152" s="0" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="153">
+      <c r="A153" s="0" t="str">
+        <f aca="false">A152</f>
+        <v>NNP-INSTITUTE</v>
+      </c>
       <c r="B153" s="0" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="C153" s="0" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="154">
+      <c r="A154" s="0" t="str">
+        <f aca="false">A153</f>
+        <v>NNP-INSTITUTE</v>
+      </c>
       <c r="B154" s="0" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="C154" s="0" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="155">
+      <c r="A155" s="0" t="str">
+        <f aca="false">A154</f>
+        <v>NNP-INSTITUTE</v>
+      </c>
       <c r="B155" s="0" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="C155" s="0" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="156">
+      <c r="A156" s="0" t="str">
+        <f aca="false">A155</f>
+        <v>NNP-INSTITUTE</v>
+      </c>
       <c r="B156" s="0" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="C156" s="0" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="157">
+      <c r="A157" s="0" t="str">
+        <f aca="false">A156</f>
+        <v>NNP-INSTITUTE</v>
+      </c>
       <c r="B157" s="0" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="C157" s="0" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="158">
+      <c r="A158" s="0" t="str">
+        <f aca="false">A157</f>
+        <v>NNP-INSTITUTE</v>
+      </c>
       <c r="B158" s="0" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="C158" s="0" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="159">
+      <c r="A159" s="0" t="str">
+        <f aca="false">A158</f>
+        <v>NNP-INSTITUTE</v>
+      </c>
       <c r="B159" s="0" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="C159" s="0" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="160">
+      <c r="A160" s="0" t="str">
+        <f aca="false">A159</f>
+        <v>NNP-INSTITUTE</v>
+      </c>
       <c r="B160" s="0" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="C160" s="0" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="161">
+      <c r="A161" s="0" t="str">
+        <f aca="false">A160</f>
+        <v>NNP-INSTITUTE</v>
+      </c>
       <c r="B161" s="0" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="C161" s="0" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="162">
+      <c r="A162" s="0" t="str">
+        <f aca="false">A161</f>
+        <v>NNP-INSTITUTE</v>
+      </c>
       <c r="B162" s="0" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="C162" s="0" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="163">
+      <c r="A163" s="0" t="str">
+        <f aca="false">A162</f>
+        <v>NNP-INSTITUTE</v>
+      </c>
       <c r="B163" s="0" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="C163" s="0" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="164">
+      <c r="A164" s="0" t="str">
+        <f aca="false">A163</f>
+        <v>NNP-INSTITUTE</v>
+      </c>
       <c r="B164" s="0" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="C164" s="0" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="165">
+      <c r="A165" s="0" t="str">
+        <f aca="false">A164</f>
+        <v>NNP-INSTITUTE</v>
+      </c>
       <c r="B165" s="0" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c r="D165" s="1"/>
       <c r="E165" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="166">
+      <c r="A166" s="0" t="str">
+        <f aca="false">A165</f>
+        <v>NNP-INSTITUTE</v>
+      </c>
       <c r="B166" s="0" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="D166" s="1"/>
       <c r="E166" s="1"/>
       <c r="F166" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="167">
+      <c r="A167" s="0" t="str">
+        <f aca="false">A166</f>
+        <v>NNP-INSTITUTE</v>
+      </c>
       <c r="B167" s="0" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="D167" s="1"/>
       <c r="E167" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="168">
+      <c r="A168" s="0" t="str">
+        <f aca="false">A167</f>
+        <v>NNP-INSTITUTE</v>
+      </c>
       <c r="B168" s="0" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="C168" s="0" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="169">
+      <c r="A169" s="0" t="str">
+        <f aca="false">A168</f>
+        <v>NNP-INSTITUTE</v>
+      </c>
       <c r="B169" s="0" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="C169" s="0" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="170">
+      <c r="A170" s="0" t="str">
+        <f aca="false">A169</f>
+        <v>NNP-INSTITUTE</v>
+      </c>
       <c r="B170" s="0" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="C170" s="0" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="171">
+      <c r="A171" s="0" t="str">
+        <f aca="false">A170</f>
+        <v>NNP-INSTITUTE</v>
+      </c>
       <c r="B171" s="0" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="C171" s="0" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="172">
+      <c r="A172" s="0" t="str">
+        <f aca="false">A171</f>
+        <v>NNP-INSTITUTE</v>
+      </c>
       <c r="B172" s="0" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="C172" s="0" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="173">
+      <c r="A173" s="0" t="str">
+        <f aca="false">A172</f>
+        <v>NNP-INSTITUTE</v>
+      </c>
       <c r="B173" s="0" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="C173" s="0" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="174">
+      <c r="A174" s="0" t="str">
+        <f aca="false">A173</f>
+        <v>NNP-INSTITUTE</v>
+      </c>
       <c r="B174" s="0" t="s">
-        <v>328</v>
+        <v>332</v>
       </c>
       <c r="C174" s="0" t="s">
-        <v>329</v>
+        <v>333</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="175">
+      <c r="A175" s="0" t="str">
+        <f aca="false">A174</f>
+        <v>NNP-INSTITUTE</v>
+      </c>
       <c r="B175" s="0" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="C175" s="0" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="176">
+      <c r="A176" s="0" t="str">
+        <f aca="false">A175</f>
+        <v>NNP-INSTITUTE</v>
+      </c>
       <c r="B176" s="0" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="C176" s="0" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="177">
+      <c r="A177" s="0" t="str">
+        <f aca="false">A176</f>
+        <v>NNP-INSTITUTE</v>
+      </c>
       <c r="B177" s="0" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="C177" s="0" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="178">
+      <c r="A178" s="0" t="str">
+        <f aca="false">A177</f>
+        <v>NNP-INSTITUTE</v>
+      </c>
       <c r="B178" s="0" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c r="C178" s="0" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="179">
+      <c r="A179" s="0" t="str">
+        <f aca="false">A178</f>
+        <v>NNP-INSTITUTE</v>
+      </c>
       <c r="B179" s="0" t="s">
-        <v>338</v>
+        <v>342</v>
       </c>
       <c r="C179" s="0" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="180">
+      <c r="A180" s="0" t="str">
+        <f aca="false">A179</f>
+        <v>NNP-INSTITUTE</v>
+      </c>
       <c r="B180" s="0" t="s">
-        <v>340</v>
+        <v>344</v>
       </c>
       <c r="C180" s="0" t="s">
-        <v>341</v>
+        <v>345</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="181">
+      <c r="A181" s="0" t="str">
+        <f aca="false">A180</f>
+        <v>NNP-INSTITUTE</v>
+      </c>
       <c r="B181" s="0" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="C181" s="0" t="s">
-        <v>343</v>
+        <v>347</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="182">
+      <c r="A182" s="0" t="str">
+        <f aca="false">A181</f>
+        <v>NNP-INSTITUTE</v>
+      </c>
       <c r="B182" s="0" t="s">
-        <v>344</v>
+        <v>348</v>
       </c>
       <c r="C182" s="0" t="s">
-        <v>345</v>
+        <v>349</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="183">
+      <c r="A183" s="0" t="str">
+        <f aca="false">A182</f>
+        <v>NNP-INSTITUTE</v>
+      </c>
       <c r="B183" s="0" t="s">
-        <v>346</v>
+        <v>350</v>
       </c>
       <c r="C183" s="0" t="s">
-        <v>347</v>
+        <v>351</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="184">
+      <c r="A184" s="0" t="str">
+        <f aca="false">A183</f>
+        <v>NNP-INSTITUTE</v>
+      </c>
       <c r="B184" s="0" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="C184" s="0" t="s">
-        <v>349</v>
+        <v>353</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="185">
+      <c r="A185" s="0" t="str">
+        <f aca="false">A184</f>
+        <v>NNP-INSTITUTE</v>
+      </c>
       <c r="B185" s="0" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="C185" s="0" t="s">
-        <v>351</v>
+        <v>355</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="186">
+      <c r="A186" s="0" t="str">
+        <f aca="false">A185</f>
+        <v>NNP-INSTITUTE</v>
+      </c>
       <c r="B186" s="0" t="s">
-        <v>352</v>
+        <v>356</v>
       </c>
       <c r="C186" s="0" t="s">
-        <v>353</v>
+        <v>357</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="188">
       <c r="B188" s="1" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="C188" s="1"/>
       <c r="D188" s="1"/>
       <c r="E188" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="189">
+      <c r="A189" s="0" t="s">
+        <v>246</v>
+      </c>
       <c r="B189" s="0" t="s">
-        <v>354</v>
+        <v>358</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="D189" s="1"/>
       <c r="E189" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="190">
+      <c r="A190" s="0" t="str">
+        <f aca="false">A189</f>
+        <v>NNP-CAMPAIGN</v>
+      </c>
       <c r="B190" s="0" t="s">
-        <v>355</v>
+        <v>359</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="D190" s="1"/>
       <c r="E190" s="1"/>
       <c r="F190" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="191">
+      <c r="A191" s="0" t="str">
+        <f aca="false">A190</f>
+        <v>NNP-CAMPAIGN</v>
+      </c>
       <c r="B191" s="0" t="s">
-        <v>356</v>
+        <v>360</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="D191" s="1"/>
       <c r="E191" s="1"/>
       <c r="F191" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="192">
+      <c r="A192" s="0" t="str">
+        <f aca="false">A191</f>
+        <v>NNP-CAMPAIGN</v>
+      </c>
       <c r="B192" s="0" t="s">
-        <v>357</v>
+        <v>361</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="D192" s="1"/>
       <c r="E192" s="1"/>
@@ -3230,21 +3743,29 @@
       <c r="H192" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="193">
+      <c r="A193" s="0" t="str">
+        <f aca="false">A192</f>
+        <v>NNP-CAMPAIGN</v>
+      </c>
       <c r="B193" s="0" t="s">
-        <v>358</v>
+        <v>362</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="D193" s="1"/>
       <c r="E193" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="194">
+      <c r="A194" s="0" t="str">
+        <f aca="false">A193</f>
+        <v>NNP-CAMPAIGN</v>
+      </c>
       <c r="B194" s="0" t="s">
-        <v>359</v>
+        <v>363</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="D194" s="1"/>
       <c r="E194" s="1"/>
@@ -3257,11 +3778,15 @@
       <c r="L194" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="195">
+      <c r="A195" s="0" t="str">
+        <f aca="false">A194</f>
+        <v>NNP-CAMPAIGN</v>
+      </c>
       <c r="B195" s="0" t="s">
-        <v>360</v>
+        <v>364</v>
       </c>
       <c r="C195" s="1" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="D195" s="1"/>
       <c r="E195" s="1"/>
@@ -3272,21 +3797,29 @@
       <c r="J195" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="196">
+      <c r="A196" s="0" t="str">
+        <f aca="false">A195</f>
+        <v>NNP-CAMPAIGN</v>
+      </c>
       <c r="B196" s="0" t="s">
-        <v>361</v>
+        <v>365</v>
       </c>
       <c r="C196" s="1" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="D196" s="1"/>
       <c r="E196" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="197">
+      <c r="A197" s="0" t="str">
+        <f aca="false">A196</f>
+        <v>NNP-CAMPAIGN</v>
+      </c>
       <c r="B197" s="0" t="s">
-        <v>362</v>
+        <v>366</v>
       </c>
       <c r="C197" s="1" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="D197" s="1"/>
       <c r="E197" s="1"/>
@@ -3295,11 +3828,15 @@
       <c r="H197" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="198">
+      <c r="A198" s="0" t="str">
+        <f aca="false">A197</f>
+        <v>NNP-CAMPAIGN</v>
+      </c>
       <c r="B198" s="0" t="s">
-        <v>363</v>
+        <v>367</v>
       </c>
       <c r="C198" s="1" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="D198" s="1"/>
       <c r="E198" s="1"/>
@@ -3307,11 +3844,15 @@
       <c r="G198" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="199">
+      <c r="A199" s="0" t="str">
+        <f aca="false">A198</f>
+        <v>NNP-CAMPAIGN</v>
+      </c>
       <c r="B199" s="0" t="s">
-        <v>364</v>
+        <v>368</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="D199" s="1"/>
       <c r="E199" s="1"/>
@@ -3319,32 +3860,44 @@
       <c r="G199" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="200">
+      <c r="A200" s="0" t="str">
+        <f aca="false">A199</f>
+        <v>NNP-CAMPAIGN</v>
+      </c>
       <c r="B200" s="0" t="s">
-        <v>365</v>
+        <v>369</v>
       </c>
       <c r="C200" s="1" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="D200" s="1"/>
       <c r="E200" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="201">
+      <c r="A201" s="0" t="str">
+        <f aca="false">A200</f>
+        <v>NNP-CAMPAIGN</v>
+      </c>
       <c r="B201" s="0" t="s">
-        <v>366</v>
+        <v>370</v>
       </c>
       <c r="C201" s="1" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="D201" s="1"/>
       <c r="E201" s="1"/>
       <c r="F201" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="202">
+      <c r="A202" s="0" t="str">
+        <f aca="false">A201</f>
+        <v>NNP-CAMPAIGN</v>
+      </c>
       <c r="B202" s="0" t="s">
-        <v>367</v>
+        <v>371</v>
       </c>
       <c r="C202" s="1" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="D202" s="1"/>
       <c r="E202" s="1"/>
@@ -3352,11 +3905,15 @@
       <c r="G202" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="203">
+      <c r="A203" s="0" t="str">
+        <f aca="false">A202</f>
+        <v>NNP-CAMPAIGN</v>
+      </c>
       <c r="B203" s="0" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="C203" s="1" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="D203" s="1"/>
       <c r="E203" s="1"/>
@@ -3364,21 +3921,29 @@
       <c r="G203" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="204">
+      <c r="A204" s="0" t="str">
+        <f aca="false">A203</f>
+        <v>NNP-CAMPAIGN</v>
+      </c>
       <c r="B204" s="0" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="C204" s="1" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="D204" s="1"/>
       <c r="E204" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="205">
+      <c r="A205" s="0" t="str">
+        <f aca="false">A204</f>
+        <v>NNP-CAMPAIGN</v>
+      </c>
       <c r="B205" s="0" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C205" s="1" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="D205" s="1"/>
       <c r="E205" s="1"/>
@@ -3386,391 +3951,421 @@
       <c r="G205" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="206">
+      <c r="A206" s="0" t="str">
+        <f aca="false">A205</f>
+        <v>NNP-CAMPAIGN</v>
+      </c>
       <c r="B206" s="0" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="C206" s="1" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="D206" s="1"/>
       <c r="E206" s="1"/>
       <c r="F206" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="207">
+      <c r="A207" s="0" t="str">
+        <f aca="false">A206</f>
+        <v>NNP-CAMPAIGN</v>
+      </c>
       <c r="B207" s="0" t="s">
-        <v>371</v>
+        <v>375</v>
       </c>
       <c r="C207" s="1" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="D207" s="1"/>
       <c r="E207" s="1"/>
       <c r="F207" s="0" t="s">
-        <v>372</v>
+        <v>376</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="208">
+      <c r="A208" s="0" t="str">
+        <f aca="false">A207</f>
+        <v>NNP-CAMPAIGN</v>
+      </c>
       <c r="B208" s="0" t="s">
-        <v>373</v>
+        <v>377</v>
       </c>
       <c r="C208" s="1" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="D208" s="1"/>
       <c r="E208" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="212">
       <c r="B212" s="0" t="s">
-        <v>374</v>
+        <v>378</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="214">
       <c r="B214" s="0" t="s">
-        <v>375</v>
+        <v>379</v>
       </c>
       <c r="C214" s="0" t="s">
-        <v>376</v>
+        <v>380</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="215">
       <c r="B215" s="0" t="s">
-        <v>377</v>
+        <v>381</v>
       </c>
       <c r="C215" s="0" t="s">
-        <v>378</v>
+        <v>382</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="216">
       <c r="B216" s="0" t="s">
-        <v>379</v>
+        <v>383</v>
       </c>
       <c r="C216" s="0" t="s">
-        <v>380</v>
+        <v>384</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="217">
       <c r="B217" s="0" t="s">
-        <v>381</v>
+        <v>385</v>
       </c>
       <c r="C217" s="0" t="s">
-        <v>382</v>
+        <v>386</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="218">
       <c r="B218" s="0" t="s">
-        <v>383</v>
+        <v>387</v>
       </c>
       <c r="C218" s="0" t="s">
-        <v>384</v>
+        <v>388</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="219">
       <c r="B219" s="0" t="s">
-        <v>385</v>
+        <v>389</v>
       </c>
       <c r="C219" s="0" t="s">
-        <v>386</v>
+        <v>390</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="220">
       <c r="B220" s="0" t="s">
-        <v>387</v>
+        <v>391</v>
       </c>
       <c r="C220" s="0" t="s">
-        <v>388</v>
+        <v>392</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="221">
       <c r="B221" s="0" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="C221" s="0" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="222">
       <c r="B222" s="0" t="s">
-        <v>391</v>
+        <v>395</v>
       </c>
       <c r="C222" s="0" t="s">
-        <v>392</v>
+        <v>396</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="225">
       <c r="B225" s="0" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="226">
       <c r="B226" s="0" t="s">
-        <v>394</v>
+        <v>398</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="227">
+      <c r="A227" s="0" t="s">
+        <v>399</v>
+      </c>
       <c r="B227" s="0" t="s">
-        <v>395</v>
+        <v>400</v>
       </c>
       <c r="C227" s="0" t="s">
-        <v>396</v>
+        <v>401</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="228">
+      <c r="A228" s="0" t="s">
+        <v>402</v>
+      </c>
       <c r="B228" s="0" t="s">
-        <v>397</v>
+        <v>403</v>
       </c>
       <c r="C228" s="0" t="s">
-        <v>398</v>
+        <v>404</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="229">
+      <c r="A229" s="0" t="s">
+        <v>405</v>
+      </c>
       <c r="B229" s="0" t="s">
-        <v>399</v>
+        <v>406</v>
       </c>
       <c r="C229" s="0" t="s">
-        <v>400</v>
+        <v>407</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="230">
+      <c r="A230" s="0" t="s">
+        <v>408</v>
+      </c>
       <c r="B230" s="0" t="s">
-        <v>401</v>
+        <v>409</v>
       </c>
       <c r="C230" s="0" t="s">
-        <v>402</v>
+        <v>410</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="231">
-      <c r="B231" s="0" t="s">
-        <v>403</v>
+      <c r="A231" s="0" t="s">
+        <v>411</v>
+      </c>
+      <c r="B231" s="1" t="s">
+        <v>412</v>
       </c>
       <c r="C231" s="0" t="s">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="232">
+      <c r="A232" s="0" t="s">
+        <v>414</v>
+      </c>
       <c r="B232" s="0" t="s">
-        <v>405</v>
+        <v>415</v>
       </c>
       <c r="C232" s="0" t="s">
-        <v>406</v>
+        <v>416</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="234">
       <c r="B234" s="0" t="s">
-        <v>407</v>
+        <v>417</v>
       </c>
       <c r="C234" s="0" t="s">
-        <v>408</v>
+        <v>418</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="235">
       <c r="B235" s="0" t="s">
-        <v>409</v>
+        <v>419</v>
       </c>
       <c r="C235" s="0" t="s">
-        <v>410</v>
+        <v>420</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="236">
       <c r="B236" s="0" t="s">
-        <v>411</v>
+        <v>421</v>
       </c>
       <c r="C236" s="0" t="s">
-        <v>410</v>
+        <v>420</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="237">
       <c r="B237" s="0" t="s">
-        <v>412</v>
+        <v>422</v>
       </c>
       <c r="C237" s="0" t="s">
-        <v>413</v>
+        <v>423</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="238">
       <c r="B238" s="0" t="s">
-        <v>414</v>
+        <v>424</v>
       </c>
       <c r="C238" s="0" t="s">
-        <v>415</v>
+        <v>425</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="239">
       <c r="B239" s="0" t="s">
-        <v>416</v>
+        <v>426</v>
       </c>
       <c r="C239" s="0" t="s">
-        <v>417</v>
+        <v>427</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="240">
       <c r="B240" s="0" t="s">
-        <v>418</v>
+        <v>428</v>
       </c>
       <c r="C240" s="0" t="s">
-        <v>419</v>
+        <v>429</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="241">
       <c r="B241" s="0" t="s">
-        <v>420</v>
+        <v>430</v>
       </c>
       <c r="C241" s="0" t="s">
-        <v>421</v>
+        <v>431</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="242">
       <c r="B242" s="0" t="s">
-        <v>422</v>
+        <v>432</v>
       </c>
       <c r="C242" s="0" t="s">
-        <v>423</v>
+        <v>433</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="243">
       <c r="B243" s="0" t="s">
-        <v>424</v>
+        <v>434</v>
       </c>
       <c r="C243" s="0" t="s">
-        <v>425</v>
+        <v>435</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="244">
       <c r="B244" s="0" t="s">
-        <v>426</v>
+        <v>436</v>
       </c>
       <c r="C244" s="0" t="s">
-        <v>427</v>
+        <v>437</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="245">
       <c r="B245" s="0" t="s">
-        <v>428</v>
+        <v>438</v>
       </c>
       <c r="C245" s="0" t="s">
-        <v>429</v>
+        <v>439</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="246">
       <c r="B246" s="0" t="s">
-        <v>430</v>
+        <v>440</v>
       </c>
       <c r="C246" s="0" t="s">
-        <v>431</v>
+        <v>441</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="247">
       <c r="B247" s="0" t="s">
-        <v>432</v>
+        <v>442</v>
       </c>
       <c r="C247" s="0" t="s">
-        <v>433</v>
+        <v>443</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="248">
       <c r="B248" s="0" t="s">
-        <v>434</v>
+        <v>444</v>
       </c>
       <c r="C248" s="0" t="s">
-        <v>435</v>
+        <v>445</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="249">
       <c r="B249" s="0" t="s">
-        <v>436</v>
+        <v>446</v>
       </c>
       <c r="C249" s="0" t="s">
-        <v>437</v>
+        <v>447</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="250">
       <c r="B250" s="0" t="s">
-        <v>438</v>
+        <v>448</v>
       </c>
       <c r="C250" s="0" t="s">
-        <v>439</v>
+        <v>449</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="251">
       <c r="B251" s="0" t="s">
-        <v>440</v>
+        <v>450</v>
       </c>
       <c r="C251" s="0" t="s">
-        <v>441</v>
+        <v>451</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="252">
       <c r="B252" s="0" t="s">
-        <v>442</v>
+        <v>452</v>
       </c>
       <c r="C252" s="0" t="s">
-        <v>443</v>
+        <v>453</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.65" outlineLevel="0" r="253">
       <c r="B253" s="0" t="s">
-        <v>444</v>
+        <v>454</v>
       </c>
       <c r="C253" s="0" t="s">
-        <v>445</v>
+        <v>455</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="254">
       <c r="B254" s="0" t="s">
-        <v>446</v>
+        <v>456</v>
       </c>
       <c r="C254" s="0" t="s">
-        <v>447</v>
+        <v>457</v>
       </c>
       <c r="E254" s="0" t="s">
-        <v>448</v>
+        <v>458</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="255">
       <c r="B255" s="0" t="s">
-        <v>449</v>
+        <v>459</v>
       </c>
       <c r="C255" s="0" t="s">
-        <v>450</v>
+        <v>460</v>
       </c>
       <c r="E255" s="0" t="s">
-        <v>448</v>
+        <v>458</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="257">
       <c r="B257" s="0" t="s">
-        <v>451</v>
+        <v>461</v>
       </c>
       <c r="C257" s="0" t="s">
-        <v>452</v>
+        <v>462</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="259">
       <c r="B259" s="0" t="s">
-        <v>453</v>
+        <v>463</v>
       </c>
       <c r="C259" s="0" t="s">
-        <v>454</v>
+        <v>464</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="260">
       <c r="B260" s="0" t="s">
-        <v>455</v>
+        <v>465</v>
       </c>
       <c r="C260" s="0" t="s">
-        <v>456</v>
+        <v>466</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="261">
       <c r="B261" s="0" t="s">
-        <v>457</v>
+        <v>467</v>
       </c>
       <c r="C261" s="0" t="s">
-        <v>458</v>
+        <v>468</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="263">
       <c r="A263" s="0" t="s">
-        <v>459</v>
+        <v>469</v>
       </c>
     </row>
   </sheetData>

</xml_diff>